<commit_message>
added in button to switch from lsip to lep changed drop down to switch b/t lsip and lep imported lsip data changed data tables to include lsip
</commit_message>
<xml_diff>
--- a/Data/2_LEPmissing/missing_leps.xlsx
+++ b/Data/2_LEPmissing/missing_leps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/2_LEPmissing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{FFE31EE7-898F-4126-9D75-02FABA5FEDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCF0A9C1-4128-4E78-802C-BD3BA2610BA0}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="8_{FFE31EE7-898F-4126-9D75-02FABA5FEDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E64F47E3-6B29-4117-AB13-8086E583E699}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{1E32C2D0-1FE1-4979-B264-7DA23B5223C8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="2" xr2:uid="{1E32C2D0-1FE1-4979-B264-7DA23B5223C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1877" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1905" uniqueCount="96">
   <si>
     <t>time_period</t>
   </si>
@@ -310,13 +310,31 @@
   </si>
   <si>
     <t xml:space="preserve">LAD21CD </t>
+  </si>
+  <si>
+    <t>LSIP21 (manually mapped)</t>
+  </si>
+  <si>
+    <t>Norfolk and Suffolk (Greater Anglia)</t>
+  </si>
+  <si>
+    <t>Heart of the South-West</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buckinghamshire </t>
+  </si>
+  <si>
+    <t>https://geoportal.statistics.gov.uk/datasets/ons::counties-and-unitary-authorities-december-2021-uk-bfc/explore?location=51.889635%2C-1.273482%2C7.00</t>
+  </si>
+  <si>
+    <t>UTLA21 map</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -340,6 +358,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -349,7 +372,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -357,15 +380,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -8428,10 +8469,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63CCF82A-C657-4D4C-8BFB-87C91102109C}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8442,7 +8483,7 @@
     <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -8458,8 +8499,11 @@
       <c r="E1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -8476,8 +8520,11 @@
         <f>INDEX(Data!C:C,MATCH(LADs!A2,Data!B:B,0))</f>
         <v>E07000201</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -8494,8 +8541,11 @@
         <f>INDEX(Data!C:C,MATCH(LADs!A3,Data!B:B,0))</f>
         <v>E07000204</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -8512,8 +8562,11 @@
         <f>INDEX(Data!C:C,MATCH(LADs!A4,Data!B:B,0))</f>
         <v>E07000205</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -8530,8 +8583,11 @@
         <f>INDEX(Data!C:C,MATCH(LADs!A5,Data!B:B,0))</f>
         <v>E07000206</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -8548,8 +8604,11 @@
         <f>INDEX(Data!C:C,MATCH(LADs!A6,Data!B:B,0))</f>
         <v>E06000028</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -8566,8 +8625,11 @@
         <f>INDEX(Data!C:C,MATCH(LADs!A7,Data!B:B,0))</f>
         <v>E07000048</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -8584,8 +8646,11 @@
         <f>INDEX(Data!C:C,MATCH(LADs!A8,Data!B:B,0))</f>
         <v>E07000049</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -8602,8 +8667,11 @@
         <f>INDEX(Data!C:C,MATCH(LADs!A9,Data!B:B,0))</f>
         <v>E07000050</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F9" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -8620,8 +8688,11 @@
         <f>INDEX(Data!C:C,MATCH(LADs!A10,Data!B:B,0))</f>
         <v>E06000029</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -8638,8 +8709,11 @@
         <f>INDEX(Data!C:C,MATCH(LADs!A11,Data!B:B,0))</f>
         <v>E07000051</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F11" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>57</v>
       </c>
@@ -8656,8 +8730,11 @@
         <f>INDEX(Data!C:C,MATCH(LADs!A12,Data!B:B,0))</f>
         <v>E07000190</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F12" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>59</v>
       </c>
@@ -8674,8 +8751,11 @@
         <f>INDEX(Data!C:C,MATCH(LADs!A13,Data!B:B,0))</f>
         <v>E07000052</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F13" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>61</v>
       </c>
@@ -8692,8 +8772,11 @@
         <f>INDEX(Data!C:C,MATCH(LADs!A14,Data!B:B,0))</f>
         <v>E07000191</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F14" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>63</v>
       </c>
@@ -8710,8 +8793,11 @@
         <f>INDEX(Data!C:C,MATCH(LADs!A15,Data!B:B,0))</f>
         <v>E07000053</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F15" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -8728,8 +8814,11 @@
         <f>INDEX(Data!C:C,MATCH(LADs!A16,Data!B:B,0))</f>
         <v>E07000004</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F16" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -8746,8 +8835,11 @@
         <f>INDEX(Data!C:C,MATCH(LADs!A17,Data!B:B,0))</f>
         <v>E07000005</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F17" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -8764,8 +8856,11 @@
         <f>INDEX(Data!C:C,MATCH(LADs!A18,Data!B:B,0))</f>
         <v>E07000006</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F18" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -8782,8 +8877,11 @@
         <f>INDEX(Data!C:C,MATCH(LADs!A19,Data!B:B,0))</f>
         <v>E07000007</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F19" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -8800,8 +8898,11 @@
         <f>INDEX(Data!C:C,MATCH(LADs!A20,Data!B:B,0))</f>
         <v>E07000150</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F20" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -8818,8 +8919,11 @@
         <f>INDEX(Data!C:C,MATCH(LADs!A21,Data!B:B,0))</f>
         <v>E07000151</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F21" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -8836,8 +8940,11 @@
         <f>INDEX(Data!C:C,MATCH(LADs!A22,Data!B:B,0))</f>
         <v>E07000152</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F22" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -8854,8 +8961,11 @@
         <f>INDEX(Data!C:C,MATCH(LADs!A23,Data!B:B,0))</f>
         <v>E07000153</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F23" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -8872,8 +8982,11 @@
         <f>INDEX(Data!C:C,MATCH(LADs!A24,Data!B:B,0))</f>
         <v>E07000154</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F24" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -8890,8 +9003,11 @@
         <f>INDEX(Data!C:C,MATCH(LADs!A25,Data!B:B,0))</f>
         <v>E07000155</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F25" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -8908,8 +9024,11 @@
         <f>INDEX(Data!C:C,MATCH(LADs!A26,Data!B:B,0))</f>
         <v>E07000156</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F26" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>65</v>
       </c>
@@ -8925,7 +9044,7 @@
         <v>z</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>65</v>
       </c>
@@ -8941,7 +9060,7 @@
         <v>z</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>65</v>
       </c>
@@ -8957,7 +9076,7 @@
         <v>z</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>65</v>
       </c>
@@ -8973,7 +9092,7 @@
         <v>z</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>65</v>
       </c>
@@ -8998,10 +9117,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD77C0D9-0462-4E4B-AB1C-15D5B966B872}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9041,12 +9160,21 @@
         <v>86</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="https://geoportal.statistics.gov.uk/documents/local-enterprise-partnerships-april-2021-map-in-england/explore" xr:uid="{7DB0B4CA-C974-4364-B47D-9AB2DA4259DC}"/>
     <hyperlink ref="B1" r:id="rId2" display="https://geoportal.statistics.gov.uk/documents/local-authority-districts-counties-and-unitary-authorities-december-2017-map-in-united-kingdom/explore" xr:uid="{EF53231C-2730-4613-A402-07FBE404C42F}"/>
     <hyperlink ref="B3" r:id="rId3" display="https://geoportal.statistics.gov.uk/documents/local-authority-districts-counties-and-unitary-authorities-december-2018-map-in-united-kingdom/explore" xr:uid="{0A50777B-E654-4839-B03F-DFFEC3B10B79}"/>
     <hyperlink ref="B4" r:id="rId4" display="https://geoportal.statistics.gov.uk/documents/local-authority-districts-counties-and-unitary-authorities-april-2019-map-in-united-kingdom/explore" xr:uid="{8FC5C104-A179-4E7C-B20C-6EC6525C8994}"/>
+    <hyperlink ref="B5" r:id="rId5" xr:uid="{C6616F6A-154E-4AE9-810D-B19109E3415D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated lookup and data files
</commit_message>
<xml_diff>
--- a/Data/2_LEPmissing/missing_leps.xlsx
+++ b/Data/2_LEPmissing/missing_leps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/2_LEPmissing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/ali_othman_education_gov_uk/Documents/Documents/lsip_dashboard/Data/2_LEPmissing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="8_{FFE31EE7-898F-4126-9D75-02FABA5FEDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E64F47E3-6B29-4117-AB13-8086E583E699}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="8_{FFE31EE7-898F-4126-9D75-02FABA5FEDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B469392-2935-4E32-BB37-CC64430B284E}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="2" xr2:uid="{1E32C2D0-1FE1-4979-B264-7DA23B5223C8}"/>
+    <workbookView xWindow="3090" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1E32C2D0-1FE1-4979-B264-7DA23B5223C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -270,9 +270,6 @@
     <t>Dorset</t>
   </si>
   <si>
-    <t>Heart of South West</t>
-  </si>
-  <si>
     <t>where to find it on the map</t>
   </si>
   <si>
@@ -315,9 +312,6 @@
     <t>LSIP21 (manually mapped)</t>
   </si>
   <si>
-    <t>Norfolk and Suffolk (Greater Anglia)</t>
-  </si>
-  <si>
     <t>Heart of the South-West</t>
   </si>
   <si>
@@ -328,6 +322,12 @@
   </si>
   <si>
     <t>UTLA21 map</t>
+  </si>
+  <si>
+    <t>Norfolk and Suffolk</t>
+  </si>
+  <si>
+    <t>Heart of the South West</t>
   </si>
 </sst>
 </file>
@@ -405,7 +405,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -8471,8 +8471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63CCF82A-C657-4D4C-8BFB-87C91102109C}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8494,13 +8494,13 @@
         <v>72</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -8521,7 +8521,7 @@
         <v>E07000201</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -8542,7 +8542,7 @@
         <v>E07000204</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -8563,7 +8563,7 @@
         <v>E07000205</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -8584,7 +8584,7 @@
         <v>E07000206</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -8598,7 +8598,7 @@
         <v>75</v>
       </c>
       <c r="D6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E6" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A6,Data!B:B,0))</f>
@@ -8619,7 +8619,7 @@
         <v>75</v>
       </c>
       <c r="D7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E7" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A7,Data!B:B,0))</f>
@@ -8640,7 +8640,7 @@
         <v>75</v>
       </c>
       <c r="D8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E8" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A8,Data!B:B,0))</f>
@@ -8661,7 +8661,7 @@
         <v>75</v>
       </c>
       <c r="D9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E9" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A9,Data!B:B,0))</f>
@@ -8682,7 +8682,7 @@
         <v>75</v>
       </c>
       <c r="D10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E10" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A10,Data!B:B,0))</f>
@@ -8703,7 +8703,7 @@
         <v>75</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E11" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A11,Data!B:B,0))</f>
@@ -8721,17 +8721,17 @@
         <v>201718</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="D12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E12" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A12,Data!B:B,0))</f>
         <v>E07000190</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -8745,7 +8745,7 @@
         <v>75</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E13" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A13,Data!B:B,0))</f>
@@ -8763,17 +8763,17 @@
         <v>201718</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="D14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E14" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A14,Data!B:B,0))</f>
         <v>E07000191</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -8787,7 +8787,7 @@
         <v>75</v>
       </c>
       <c r="D15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E15" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A15,Data!B:B,0))</f>
@@ -8805,17 +8805,17 @@
         <v>201819</v>
       </c>
       <c r="C16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E16" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A16,Data!B:B,0))</f>
         <v>E07000004</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -8826,17 +8826,17 @@
         <v>201819</v>
       </c>
       <c r="C17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" t="s">
         <v>83</v>
-      </c>
-      <c r="D17" t="s">
-        <v>84</v>
       </c>
       <c r="E17" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A17,Data!B:B,0))</f>
         <v>E07000005</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -8847,17 +8847,17 @@
         <v>201819</v>
       </c>
       <c r="C18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" t="s">
         <v>83</v>
-      </c>
-      <c r="D18" t="s">
-        <v>84</v>
       </c>
       <c r="E18" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A18,Data!B:B,0))</f>
         <v>E07000006</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -8868,17 +8868,17 @@
         <v>201819</v>
       </c>
       <c r="C19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" t="s">
         <v>83</v>
-      </c>
-      <c r="D19" t="s">
-        <v>84</v>
       </c>
       <c r="E19" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A19,Data!B:B,0))</f>
         <v>E07000007</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -8889,17 +8889,17 @@
         <v>201920</v>
       </c>
       <c r="C20" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" t="s">
         <v>87</v>
-      </c>
-      <c r="D20" t="s">
-        <v>88</v>
       </c>
       <c r="E20" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A20,Data!B:B,0))</f>
         <v>E07000150</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
@@ -8910,17 +8910,17 @@
         <v>201920</v>
       </c>
       <c r="C21" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" t="s">
         <v>87</v>
-      </c>
-      <c r="D21" t="s">
-        <v>88</v>
       </c>
       <c r="E21" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A21,Data!B:B,0))</f>
         <v>E07000151</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
@@ -8931,17 +8931,17 @@
         <v>201920</v>
       </c>
       <c r="C22" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" t="s">
         <v>87</v>
-      </c>
-      <c r="D22" t="s">
-        <v>88</v>
       </c>
       <c r="E22" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A22,Data!B:B,0))</f>
         <v>E07000152</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
@@ -8952,17 +8952,17 @@
         <v>201920</v>
       </c>
       <c r="C23" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" t="s">
         <v>87</v>
-      </c>
-      <c r="D23" t="s">
-        <v>88</v>
       </c>
       <c r="E23" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A23,Data!B:B,0))</f>
         <v>E07000153</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
@@ -8973,17 +8973,17 @@
         <v>201920</v>
       </c>
       <c r="C24" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" t="s">
         <v>87</v>
-      </c>
-      <c r="D24" t="s">
-        <v>88</v>
       </c>
       <c r="E24" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A24,Data!B:B,0))</f>
         <v>E07000154</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
@@ -8994,17 +8994,17 @@
         <v>201920</v>
       </c>
       <c r="C25" t="s">
+        <v>86</v>
+      </c>
+      <c r="D25" t="s">
         <v>87</v>
-      </c>
-      <c r="D25" t="s">
-        <v>88</v>
       </c>
       <c r="E25" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A25,Data!B:B,0))</f>
         <v>E07000155</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
@@ -9015,17 +9015,17 @@
         <v>201920</v>
       </c>
       <c r="C26" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26" t="s">
         <v>87</v>
-      </c>
-      <c r="D26" t="s">
-        <v>88</v>
       </c>
       <c r="E26" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A26,Data!B:B,0))</f>
         <v>E07000156</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
@@ -9119,7 +9119,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD77C0D9-0462-4E4B-AB1C-15D5B966B872}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -9146,26 +9146,26 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>